<commit_message>
completed account terms tests
</commit_message>
<xml_diff>
--- a/validation/insurance_account_test_case_list.xlsx
+++ b/validation/insurance_account_test_case_list.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_859-test-cases\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_fm_pol_cov_tests\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B5B730-56A5-4BD5-B754-A09088B190EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAA8CB0-154E-4A35-81F4-A7702EF2E8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="4110" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="780" windowWidth="22044" windowHeight="12384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="insurance_account" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="125">
   <si>
     <t>LocDed6All</t>
   </si>
@@ -352,9 +365,6 @@
     <t>acc96</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>Key</t>
   </si>
   <si>
@@ -380,6 +390,24 @@
   </si>
   <si>
     <t>Description of units in insurance_account test</t>
+  </si>
+  <si>
+    <t>AccParticipation</t>
+  </si>
+  <si>
+    <t>acc97</t>
+  </si>
+  <si>
+    <t>acc98</t>
+  </si>
+  <si>
+    <t>acc99</t>
+  </si>
+  <si>
+    <t>acc100</t>
+  </si>
+  <si>
+    <t>complete</t>
   </si>
 </sst>
 </file>
@@ -1226,35 +1254,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O98"/>
+  <dimension ref="A1:P102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.53125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.9296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1284,19 +1313,22 @@
         <v>11</v>
       </c>
       <c r="K2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>6</v>
       </c>
-      <c r="N2" t="s">
-        <v>111</v>
-      </c>
       <c r="O2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+      <c r="P2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1321,17 +1353,17 @@
       <c r="J3" t="s">
         <v>7</v>
       </c>
-      <c r="L3" t="s">
-        <v>110</v>
-      </c>
-      <c r="N3" t="s">
-        <v>112</v>
+      <c r="M3" t="s">
+        <v>124</v>
       </c>
       <c r="O3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+        <v>111</v>
+      </c>
+      <c r="P3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1356,17 +1388,17 @@
       <c r="J4" t="s">
         <v>9</v>
       </c>
-      <c r="L4" t="s">
-        <v>110</v>
-      </c>
-      <c r="N4" t="s">
-        <v>7</v>
+      <c r="M4" t="s">
+        <v>124</v>
       </c>
       <c r="O4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="P4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1391,17 +1423,17 @@
       <c r="J5" t="s">
         <v>8</v>
       </c>
-      <c r="L5" t="s">
-        <v>110</v>
-      </c>
-      <c r="N5" t="s">
-        <v>8</v>
+      <c r="M5" t="s">
+        <v>124</v>
       </c>
       <c r="O5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="P5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1423,17 +1455,17 @@
       <c r="I6" t="s">
         <v>7</v>
       </c>
-      <c r="L6" t="s">
-        <v>110</v>
-      </c>
-      <c r="N6" t="s">
-        <v>9</v>
+      <c r="M6" t="s">
+        <v>124</v>
       </c>
       <c r="O6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="P6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1458,11 +1490,11 @@
       <c r="J7" t="s">
         <v>7</v>
       </c>
-      <c r="L7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1487,11 +1519,11 @@
       <c r="J8" t="s">
         <v>9</v>
       </c>
-      <c r="L8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1516,11 +1548,11 @@
       <c r="J9" t="s">
         <v>8</v>
       </c>
-      <c r="L9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1542,11 +1574,11 @@
       <c r="I10" t="s">
         <v>7</v>
       </c>
-      <c r="L10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1571,11 +1603,11 @@
       <c r="J11" t="s">
         <v>7</v>
       </c>
-      <c r="L11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1600,11 +1632,11 @@
       <c r="J12" t="s">
         <v>9</v>
       </c>
-      <c r="L12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1629,11 +1661,11 @@
       <c r="J13" t="s">
         <v>8</v>
       </c>
-      <c r="L13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1655,11 +1687,11 @@
       <c r="I14" t="s">
         <v>7</v>
       </c>
-      <c r="L14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1681,11 +1713,11 @@
       <c r="J15" t="s">
         <v>7</v>
       </c>
-      <c r="L15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1707,11 +1739,11 @@
       <c r="J16" t="s">
         <v>9</v>
       </c>
-      <c r="L16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1733,11 +1765,11 @@
       <c r="J17" t="s">
         <v>8</v>
       </c>
-      <c r="L17" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1756,11 +1788,11 @@
       <c r="H18" t="s">
         <v>7</v>
       </c>
-      <c r="L18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1782,11 +1814,11 @@
       <c r="J19" t="s">
         <v>7</v>
       </c>
-      <c r="L19" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1808,11 +1840,11 @@
       <c r="J20" t="s">
         <v>9</v>
       </c>
-      <c r="L20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1834,11 +1866,11 @@
       <c r="J21" t="s">
         <v>8</v>
       </c>
-      <c r="L21" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1857,11 +1889,11 @@
       <c r="H22" t="s">
         <v>7</v>
       </c>
-      <c r="L22" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1883,11 +1915,11 @@
       <c r="J23" t="s">
         <v>7</v>
       </c>
-      <c r="L23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1909,11 +1941,11 @@
       <c r="J24" t="s">
         <v>9</v>
       </c>
-      <c r="L24" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1935,11 +1967,11 @@
       <c r="J25" t="s">
         <v>8</v>
       </c>
-      <c r="L25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1958,11 +1990,11 @@
       <c r="H26" t="s">
         <v>7</v>
       </c>
-      <c r="L26" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1984,11 +2016,11 @@
       <c r="J27" t="s">
         <v>7</v>
       </c>
-      <c r="L27" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -2010,11 +2042,11 @@
       <c r="J28" t="s">
         <v>9</v>
       </c>
-      <c r="L28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -2036,11 +2068,11 @@
       <c r="J29" t="s">
         <v>8</v>
       </c>
-      <c r="L29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2059,11 +2091,11 @@
       <c r="I30" t="s">
         <v>7</v>
       </c>
-      <c r="L30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2085,11 +2117,11 @@
       <c r="J31" t="s">
         <v>7</v>
       </c>
-      <c r="L31" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2111,11 +2143,11 @@
       <c r="J32" t="s">
         <v>9</v>
       </c>
-      <c r="L32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -2137,11 +2169,11 @@
       <c r="J33" t="s">
         <v>8</v>
       </c>
-      <c r="L33" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -2160,11 +2192,11 @@
       <c r="I34" t="s">
         <v>7</v>
       </c>
-      <c r="L34" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -2186,11 +2218,11 @@
       <c r="J35" t="s">
         <v>7</v>
       </c>
-      <c r="L35" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -2212,11 +2244,11 @@
       <c r="J36" t="s">
         <v>9</v>
       </c>
-      <c r="L36" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -2238,11 +2270,11 @@
       <c r="J37" t="s">
         <v>8</v>
       </c>
-      <c r="L37" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -2261,11 +2293,11 @@
       <c r="I38" t="s">
         <v>7</v>
       </c>
-      <c r="L38" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -2284,11 +2316,11 @@
       <c r="J39" t="s">
         <v>7</v>
       </c>
-      <c r="L39" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M39" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -2307,11 +2339,11 @@
       <c r="J40" t="s">
         <v>9</v>
       </c>
-      <c r="L40" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M40" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -2330,11 +2362,11 @@
       <c r="J41" t="s">
         <v>8</v>
       </c>
-      <c r="L41" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -2350,11 +2382,11 @@
       <c r="G42" t="s">
         <v>8</v>
       </c>
-      <c r="L42" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M42" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -2373,11 +2405,11 @@
       <c r="J43" t="s">
         <v>7</v>
       </c>
-      <c r="L43" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -2396,11 +2428,11 @@
       <c r="J44" t="s">
         <v>9</v>
       </c>
-      <c r="L44" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M44" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -2419,11 +2451,11 @@
       <c r="J45" t="s">
         <v>8</v>
       </c>
-      <c r="L45" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -2439,11 +2471,11 @@
       <c r="G46" t="s">
         <v>9</v>
       </c>
-      <c r="L46" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -2462,11 +2494,11 @@
       <c r="J47" t="s">
         <v>7</v>
       </c>
-      <c r="L47" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M47" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -2485,11 +2517,11 @@
       <c r="J48" t="s">
         <v>9</v>
       </c>
-      <c r="L48" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M48" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -2508,11 +2540,11 @@
       <c r="J49" t="s">
         <v>8</v>
       </c>
-      <c r="L49" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M49" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -2528,11 +2560,11 @@
       <c r="G50" t="s">
         <v>7</v>
       </c>
-      <c r="L50" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M50" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -2560,11 +2592,11 @@
       <c r="J51" t="s">
         <v>7</v>
       </c>
-      <c r="L51" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -2592,11 +2624,11 @@
       <c r="J52" t="s">
         <v>9</v>
       </c>
-      <c r="L52" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M52" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -2624,11 +2656,11 @@
       <c r="J53" t="s">
         <v>8</v>
       </c>
-      <c r="L53" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -2653,11 +2685,11 @@
       <c r="I54" t="s">
         <v>7</v>
       </c>
-      <c r="L54" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -2685,11 +2717,11 @@
       <c r="J55" t="s">
         <v>7</v>
       </c>
-      <c r="L55" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -2717,11 +2749,11 @@
       <c r="J56" t="s">
         <v>9</v>
       </c>
-      <c r="L56" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M56" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -2749,11 +2781,11 @@
       <c r="J57" t="s">
         <v>8</v>
       </c>
-      <c r="L57" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>69</v>
       </c>
@@ -2778,11 +2810,11 @@
       <c r="I58" t="s">
         <v>7</v>
       </c>
-      <c r="L58" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M58" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -2810,11 +2842,11 @@
       <c r="J59" t="s">
         <v>7</v>
       </c>
-      <c r="L59" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M59" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>71</v>
       </c>
@@ -2842,11 +2874,11 @@
       <c r="J60" t="s">
         <v>9</v>
       </c>
-      <c r="L60" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>72</v>
       </c>
@@ -2874,11 +2906,11 @@
       <c r="J61" t="s">
         <v>8</v>
       </c>
-      <c r="L61" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M61" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>73</v>
       </c>
@@ -2903,11 +2935,11 @@
       <c r="I62" t="s">
         <v>7</v>
       </c>
-      <c r="L62" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M62" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>74</v>
       </c>
@@ -2932,11 +2964,11 @@
       <c r="J63" t="s">
         <v>7</v>
       </c>
-      <c r="L63" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M63" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>75</v>
       </c>
@@ -2961,11 +2993,11 @@
       <c r="J64" t="s">
         <v>9</v>
       </c>
-      <c r="L64" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M64" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>76</v>
       </c>
@@ -2990,11 +3022,11 @@
       <c r="J65" t="s">
         <v>8</v>
       </c>
-      <c r="L65" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M65" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>77</v>
       </c>
@@ -3016,11 +3048,11 @@
       <c r="H66" t="s">
         <v>7</v>
       </c>
-      <c r="L66" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M66" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -3045,11 +3077,11 @@
       <c r="J67" t="s">
         <v>7</v>
       </c>
-      <c r="L67" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M67" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -3074,11 +3106,11 @@
       <c r="J68" t="s">
         <v>9</v>
       </c>
-      <c r="L68" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M68" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -3103,11 +3135,11 @@
       <c r="J69" t="s">
         <v>8</v>
       </c>
-      <c r="L69" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M69" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>81</v>
       </c>
@@ -3129,11 +3161,11 @@
       <c r="H70" t="s">
         <v>7</v>
       </c>
-      <c r="L70" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M70" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -3158,11 +3190,11 @@
       <c r="J71" t="s">
         <v>7</v>
       </c>
-      <c r="L71" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M71" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -3187,11 +3219,11 @@
       <c r="J72" t="s">
         <v>9</v>
       </c>
-      <c r="L72" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M72" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>84</v>
       </c>
@@ -3216,11 +3248,11 @@
       <c r="J73" t="s">
         <v>8</v>
       </c>
-      <c r="L73" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M73" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -3242,11 +3274,11 @@
       <c r="H74" t="s">
         <v>7</v>
       </c>
-      <c r="L74" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M74" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>86</v>
       </c>
@@ -3271,11 +3303,11 @@
       <c r="J75" t="s">
         <v>7</v>
       </c>
-      <c r="L75" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M75" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>87</v>
       </c>
@@ -3300,11 +3332,11 @@
       <c r="J76" t="s">
         <v>9</v>
       </c>
-      <c r="L76" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M76" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>88</v>
       </c>
@@ -3329,11 +3361,11 @@
       <c r="J77" t="s">
         <v>8</v>
       </c>
-      <c r="L77" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M77" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>89</v>
       </c>
@@ -3355,11 +3387,11 @@
       <c r="I78" t="s">
         <v>7</v>
       </c>
-      <c r="L78" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M78" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>90</v>
       </c>
@@ -3384,11 +3416,11 @@
       <c r="J79" t="s">
         <v>7</v>
       </c>
-      <c r="L79" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M79" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>91</v>
       </c>
@@ -3413,11 +3445,11 @@
       <c r="J80" t="s">
         <v>9</v>
       </c>
-      <c r="L80" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M80" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>92</v>
       </c>
@@ -3442,11 +3474,11 @@
       <c r="J81" t="s">
         <v>8</v>
       </c>
-      <c r="L81" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M81" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>93</v>
       </c>
@@ -3468,11 +3500,11 @@
       <c r="I82" t="s">
         <v>7</v>
       </c>
-      <c r="L82" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M82" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>94</v>
       </c>
@@ -3497,11 +3529,11 @@
       <c r="J83" t="s">
         <v>7</v>
       </c>
-      <c r="L83" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M83" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>95</v>
       </c>
@@ -3526,11 +3558,11 @@
       <c r="J84" t="s">
         <v>9</v>
       </c>
-      <c r="L84" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M84" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>96</v>
       </c>
@@ -3555,11 +3587,11 @@
       <c r="J85" t="s">
         <v>8</v>
       </c>
-      <c r="L85" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M85" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>97</v>
       </c>
@@ -3581,11 +3613,11 @@
       <c r="I86" t="s">
         <v>7</v>
       </c>
-      <c r="L86" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M86" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>98</v>
       </c>
@@ -3607,11 +3639,11 @@
       <c r="J87" t="s">
         <v>7</v>
       </c>
-      <c r="L87" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M87" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>99</v>
       </c>
@@ -3633,11 +3665,11 @@
       <c r="J88" t="s">
         <v>9</v>
       </c>
-      <c r="L88" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M88" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>100</v>
       </c>
@@ -3659,11 +3691,11 @@
       <c r="J89" t="s">
         <v>8</v>
       </c>
-      <c r="L89" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M89" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>101</v>
       </c>
@@ -3682,11 +3714,11 @@
       <c r="G90" t="s">
         <v>8</v>
       </c>
-      <c r="L90" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M90" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>102</v>
       </c>
@@ -3708,11 +3740,11 @@
       <c r="J91" t="s">
         <v>7</v>
       </c>
-      <c r="L91" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M91" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>103</v>
       </c>
@@ -3734,11 +3766,11 @@
       <c r="J92" t="s">
         <v>9</v>
       </c>
-      <c r="L92" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M92" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>104</v>
       </c>
@@ -3760,11 +3792,11 @@
       <c r="J93" t="s">
         <v>8</v>
       </c>
-      <c r="L93" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M93" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>105</v>
       </c>
@@ -3783,11 +3815,11 @@
       <c r="G94" t="s">
         <v>9</v>
       </c>
-      <c r="L94" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M94" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>106</v>
       </c>
@@ -3809,11 +3841,11 @@
       <c r="J95" t="s">
         <v>7</v>
       </c>
-      <c r="L95" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M95" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>107</v>
       </c>
@@ -3835,11 +3867,11 @@
       <c r="J96" t="s">
         <v>9</v>
       </c>
-      <c r="L96" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M96" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>108</v>
       </c>
@@ -3861,11 +3893,11 @@
       <c r="J97" t="s">
         <v>8</v>
       </c>
-      <c r="L97" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M97" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>109</v>
       </c>
@@ -3884,8 +3916,136 @@
       <c r="G98" t="s">
         <v>7</v>
       </c>
-      <c r="L98" t="s">
-        <v>110</v>
+      <c r="M98" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>120</v>
+      </c>
+      <c r="D99" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99" t="s">
+        <v>7</v>
+      </c>
+      <c r="F99" t="s">
+        <v>8</v>
+      </c>
+      <c r="G99" t="s">
+        <v>8</v>
+      </c>
+      <c r="H99" t="s">
+        <v>7</v>
+      </c>
+      <c r="I99" t="s">
+        <v>7</v>
+      </c>
+      <c r="J99" t="s">
+        <v>7</v>
+      </c>
+      <c r="K99" t="s">
+        <v>8</v>
+      </c>
+      <c r="M99" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>121</v>
+      </c>
+      <c r="D100" t="s">
+        <v>7</v>
+      </c>
+      <c r="E100" t="s">
+        <v>7</v>
+      </c>
+      <c r="F100" t="s">
+        <v>8</v>
+      </c>
+      <c r="G100" t="s">
+        <v>8</v>
+      </c>
+      <c r="H100" t="s">
+        <v>7</v>
+      </c>
+      <c r="I100" t="s">
+        <v>7</v>
+      </c>
+      <c r="K100" t="s">
+        <v>8</v>
+      </c>
+      <c r="M100" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>122</v>
+      </c>
+      <c r="B101" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" t="s">
+        <v>7</v>
+      </c>
+      <c r="E101" t="s">
+        <v>7</v>
+      </c>
+      <c r="F101" t="s">
+        <v>8</v>
+      </c>
+      <c r="G101" t="s">
+        <v>8</v>
+      </c>
+      <c r="H101" t="s">
+        <v>7</v>
+      </c>
+      <c r="I101" t="s">
+        <v>7</v>
+      </c>
+      <c r="J101" t="s">
+        <v>7</v>
+      </c>
+      <c r="K101" t="s">
+        <v>8</v>
+      </c>
+      <c r="M101" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>123</v>
+      </c>
+      <c r="B102" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102" t="s">
+        <v>7</v>
+      </c>
+      <c r="E102" t="s">
+        <v>7</v>
+      </c>
+      <c r="F102" t="s">
+        <v>8</v>
+      </c>
+      <c r="G102" t="s">
+        <v>8</v>
+      </c>
+      <c r="H102" t="s">
+        <v>7</v>
+      </c>
+      <c r="I102" t="s">
+        <v>7</v>
+      </c>
+      <c r="K102" t="s">
+        <v>8</v>
+      </c>
+      <c r="M102" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tests for condition coverages 1-5 financial terms (#1407)
* added test cases for conditions

* updated expected for policy coverage tests

* updated units for policy coverage tests

* set status to complete for all units

* added test cases 97-100 and updated units

* completed account terms tests

* fix empty cond priority issue

---------

Co-authored-by: sstruzik <stephane.struzik@gmail.com>
Co-authored-by: Sam Gamble <hexadessa@gmail.com>
</commit_message>
<xml_diff>
--- a/validation/insurance_account_test_case_list.xlsx
+++ b/validation/insurance_account_test_case_list.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_859-test-cases\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_fm_pol_cov_tests\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B5B730-56A5-4BD5-B754-A09088B190EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAA8CB0-154E-4A35-81F4-A7702EF2E8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="4110" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="780" windowWidth="22044" windowHeight="12384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="insurance_account" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="125">
   <si>
     <t>LocDed6All</t>
   </si>
@@ -352,9 +365,6 @@
     <t>acc96</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>Key</t>
   </si>
   <si>
@@ -380,6 +390,24 @@
   </si>
   <si>
     <t>Description of units in insurance_account test</t>
+  </si>
+  <si>
+    <t>AccParticipation</t>
+  </si>
+  <si>
+    <t>acc97</t>
+  </si>
+  <si>
+    <t>acc98</t>
+  </si>
+  <si>
+    <t>acc99</t>
+  </si>
+  <si>
+    <t>acc100</t>
+  </si>
+  <si>
+    <t>complete</t>
   </si>
 </sst>
 </file>
@@ -1226,35 +1254,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O98"/>
+  <dimension ref="A1:P102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.53125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.9296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1284,19 +1313,22 @@
         <v>11</v>
       </c>
       <c r="K2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>6</v>
       </c>
-      <c r="N2" t="s">
-        <v>111</v>
-      </c>
       <c r="O2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+      <c r="P2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1321,17 +1353,17 @@
       <c r="J3" t="s">
         <v>7</v>
       </c>
-      <c r="L3" t="s">
-        <v>110</v>
-      </c>
-      <c r="N3" t="s">
-        <v>112</v>
+      <c r="M3" t="s">
+        <v>124</v>
       </c>
       <c r="O3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+        <v>111</v>
+      </c>
+      <c r="P3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1356,17 +1388,17 @@
       <c r="J4" t="s">
         <v>9</v>
       </c>
-      <c r="L4" t="s">
-        <v>110</v>
-      </c>
-      <c r="N4" t="s">
-        <v>7</v>
+      <c r="M4" t="s">
+        <v>124</v>
       </c>
       <c r="O4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="P4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1391,17 +1423,17 @@
       <c r="J5" t="s">
         <v>8</v>
       </c>
-      <c r="L5" t="s">
-        <v>110</v>
-      </c>
-      <c r="N5" t="s">
-        <v>8</v>
+      <c r="M5" t="s">
+        <v>124</v>
       </c>
       <c r="O5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="P5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1423,17 +1455,17 @@
       <c r="I6" t="s">
         <v>7</v>
       </c>
-      <c r="L6" t="s">
-        <v>110</v>
-      </c>
-      <c r="N6" t="s">
-        <v>9</v>
+      <c r="M6" t="s">
+        <v>124</v>
       </c>
       <c r="O6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="P6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1458,11 +1490,11 @@
       <c r="J7" t="s">
         <v>7</v>
       </c>
-      <c r="L7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1487,11 +1519,11 @@
       <c r="J8" t="s">
         <v>9</v>
       </c>
-      <c r="L8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1516,11 +1548,11 @@
       <c r="J9" t="s">
         <v>8</v>
       </c>
-      <c r="L9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1542,11 +1574,11 @@
       <c r="I10" t="s">
         <v>7</v>
       </c>
-      <c r="L10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1571,11 +1603,11 @@
       <c r="J11" t="s">
         <v>7</v>
       </c>
-      <c r="L11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1600,11 +1632,11 @@
       <c r="J12" t="s">
         <v>9</v>
       </c>
-      <c r="L12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1629,11 +1661,11 @@
       <c r="J13" t="s">
         <v>8</v>
       </c>
-      <c r="L13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1655,11 +1687,11 @@
       <c r="I14" t="s">
         <v>7</v>
       </c>
-      <c r="L14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1681,11 +1713,11 @@
       <c r="J15" t="s">
         <v>7</v>
       </c>
-      <c r="L15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1707,11 +1739,11 @@
       <c r="J16" t="s">
         <v>9</v>
       </c>
-      <c r="L16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1733,11 +1765,11 @@
       <c r="J17" t="s">
         <v>8</v>
       </c>
-      <c r="L17" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1756,11 +1788,11 @@
       <c r="H18" t="s">
         <v>7</v>
       </c>
-      <c r="L18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1782,11 +1814,11 @@
       <c r="J19" t="s">
         <v>7</v>
       </c>
-      <c r="L19" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1808,11 +1840,11 @@
       <c r="J20" t="s">
         <v>9</v>
       </c>
-      <c r="L20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1834,11 +1866,11 @@
       <c r="J21" t="s">
         <v>8</v>
       </c>
-      <c r="L21" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1857,11 +1889,11 @@
       <c r="H22" t="s">
         <v>7</v>
       </c>
-      <c r="L22" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1883,11 +1915,11 @@
       <c r="J23" t="s">
         <v>7</v>
       </c>
-      <c r="L23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1909,11 +1941,11 @@
       <c r="J24" t="s">
         <v>9</v>
       </c>
-      <c r="L24" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1935,11 +1967,11 @@
       <c r="J25" t="s">
         <v>8</v>
       </c>
-      <c r="L25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1958,11 +1990,11 @@
       <c r="H26" t="s">
         <v>7</v>
       </c>
-      <c r="L26" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1984,11 +2016,11 @@
       <c r="J27" t="s">
         <v>7</v>
       </c>
-      <c r="L27" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -2010,11 +2042,11 @@
       <c r="J28" t="s">
         <v>9</v>
       </c>
-      <c r="L28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -2036,11 +2068,11 @@
       <c r="J29" t="s">
         <v>8</v>
       </c>
-      <c r="L29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2059,11 +2091,11 @@
       <c r="I30" t="s">
         <v>7</v>
       </c>
-      <c r="L30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2085,11 +2117,11 @@
       <c r="J31" t="s">
         <v>7</v>
       </c>
-      <c r="L31" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2111,11 +2143,11 @@
       <c r="J32" t="s">
         <v>9</v>
       </c>
-      <c r="L32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -2137,11 +2169,11 @@
       <c r="J33" t="s">
         <v>8</v>
       </c>
-      <c r="L33" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -2160,11 +2192,11 @@
       <c r="I34" t="s">
         <v>7</v>
       </c>
-      <c r="L34" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -2186,11 +2218,11 @@
       <c r="J35" t="s">
         <v>7</v>
       </c>
-      <c r="L35" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -2212,11 +2244,11 @@
       <c r="J36" t="s">
         <v>9</v>
       </c>
-      <c r="L36" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -2238,11 +2270,11 @@
       <c r="J37" t="s">
         <v>8</v>
       </c>
-      <c r="L37" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -2261,11 +2293,11 @@
       <c r="I38" t="s">
         <v>7</v>
       </c>
-      <c r="L38" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -2284,11 +2316,11 @@
       <c r="J39" t="s">
         <v>7</v>
       </c>
-      <c r="L39" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M39" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -2307,11 +2339,11 @@
       <c r="J40" t="s">
         <v>9</v>
       </c>
-      <c r="L40" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M40" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -2330,11 +2362,11 @@
       <c r="J41" t="s">
         <v>8</v>
       </c>
-      <c r="L41" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -2350,11 +2382,11 @@
       <c r="G42" t="s">
         <v>8</v>
       </c>
-      <c r="L42" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M42" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -2373,11 +2405,11 @@
       <c r="J43" t="s">
         <v>7</v>
       </c>
-      <c r="L43" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -2396,11 +2428,11 @@
       <c r="J44" t="s">
         <v>9</v>
       </c>
-      <c r="L44" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M44" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -2419,11 +2451,11 @@
       <c r="J45" t="s">
         <v>8</v>
       </c>
-      <c r="L45" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -2439,11 +2471,11 @@
       <c r="G46" t="s">
         <v>9</v>
       </c>
-      <c r="L46" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -2462,11 +2494,11 @@
       <c r="J47" t="s">
         <v>7</v>
       </c>
-      <c r="L47" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M47" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -2485,11 +2517,11 @@
       <c r="J48" t="s">
         <v>9</v>
       </c>
-      <c r="L48" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M48" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -2508,11 +2540,11 @@
       <c r="J49" t="s">
         <v>8</v>
       </c>
-      <c r="L49" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M49" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -2528,11 +2560,11 @@
       <c r="G50" t="s">
         <v>7</v>
       </c>
-      <c r="L50" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M50" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -2560,11 +2592,11 @@
       <c r="J51" t="s">
         <v>7</v>
       </c>
-      <c r="L51" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -2592,11 +2624,11 @@
       <c r="J52" t="s">
         <v>9</v>
       </c>
-      <c r="L52" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M52" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -2624,11 +2656,11 @@
       <c r="J53" t="s">
         <v>8</v>
       </c>
-      <c r="L53" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -2653,11 +2685,11 @@
       <c r="I54" t="s">
         <v>7</v>
       </c>
-      <c r="L54" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -2685,11 +2717,11 @@
       <c r="J55" t="s">
         <v>7</v>
       </c>
-      <c r="L55" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -2717,11 +2749,11 @@
       <c r="J56" t="s">
         <v>9</v>
       </c>
-      <c r="L56" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M56" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -2749,11 +2781,11 @@
       <c r="J57" t="s">
         <v>8</v>
       </c>
-      <c r="L57" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>69</v>
       </c>
@@ -2778,11 +2810,11 @@
       <c r="I58" t="s">
         <v>7</v>
       </c>
-      <c r="L58" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M58" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -2810,11 +2842,11 @@
       <c r="J59" t="s">
         <v>7</v>
       </c>
-      <c r="L59" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M59" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>71</v>
       </c>
@@ -2842,11 +2874,11 @@
       <c r="J60" t="s">
         <v>9</v>
       </c>
-      <c r="L60" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>72</v>
       </c>
@@ -2874,11 +2906,11 @@
       <c r="J61" t="s">
         <v>8</v>
       </c>
-      <c r="L61" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M61" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>73</v>
       </c>
@@ -2903,11 +2935,11 @@
       <c r="I62" t="s">
         <v>7</v>
       </c>
-      <c r="L62" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M62" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>74</v>
       </c>
@@ -2932,11 +2964,11 @@
       <c r="J63" t="s">
         <v>7</v>
       </c>
-      <c r="L63" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M63" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>75</v>
       </c>
@@ -2961,11 +2993,11 @@
       <c r="J64" t="s">
         <v>9</v>
       </c>
-      <c r="L64" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M64" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>76</v>
       </c>
@@ -2990,11 +3022,11 @@
       <c r="J65" t="s">
         <v>8</v>
       </c>
-      <c r="L65" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M65" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>77</v>
       </c>
@@ -3016,11 +3048,11 @@
       <c r="H66" t="s">
         <v>7</v>
       </c>
-      <c r="L66" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M66" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -3045,11 +3077,11 @@
       <c r="J67" t="s">
         <v>7</v>
       </c>
-      <c r="L67" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M67" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -3074,11 +3106,11 @@
       <c r="J68" t="s">
         <v>9</v>
       </c>
-      <c r="L68" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M68" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -3103,11 +3135,11 @@
       <c r="J69" t="s">
         <v>8</v>
       </c>
-      <c r="L69" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M69" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>81</v>
       </c>
@@ -3129,11 +3161,11 @@
       <c r="H70" t="s">
         <v>7</v>
       </c>
-      <c r="L70" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M70" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -3158,11 +3190,11 @@
       <c r="J71" t="s">
         <v>7</v>
       </c>
-      <c r="L71" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M71" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -3187,11 +3219,11 @@
       <c r="J72" t="s">
         <v>9</v>
       </c>
-      <c r="L72" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M72" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>84</v>
       </c>
@@ -3216,11 +3248,11 @@
       <c r="J73" t="s">
         <v>8</v>
       </c>
-      <c r="L73" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M73" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -3242,11 +3274,11 @@
       <c r="H74" t="s">
         <v>7</v>
       </c>
-      <c r="L74" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M74" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>86</v>
       </c>
@@ -3271,11 +3303,11 @@
       <c r="J75" t="s">
         <v>7</v>
       </c>
-      <c r="L75" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M75" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>87</v>
       </c>
@@ -3300,11 +3332,11 @@
       <c r="J76" t="s">
         <v>9</v>
       </c>
-      <c r="L76" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M76" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>88</v>
       </c>
@@ -3329,11 +3361,11 @@
       <c r="J77" t="s">
         <v>8</v>
       </c>
-      <c r="L77" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M77" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>89</v>
       </c>
@@ -3355,11 +3387,11 @@
       <c r="I78" t="s">
         <v>7</v>
       </c>
-      <c r="L78" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M78" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>90</v>
       </c>
@@ -3384,11 +3416,11 @@
       <c r="J79" t="s">
         <v>7</v>
       </c>
-      <c r="L79" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M79" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>91</v>
       </c>
@@ -3413,11 +3445,11 @@
       <c r="J80" t="s">
         <v>9</v>
       </c>
-      <c r="L80" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M80" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>92</v>
       </c>
@@ -3442,11 +3474,11 @@
       <c r="J81" t="s">
         <v>8</v>
       </c>
-      <c r="L81" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M81" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>93</v>
       </c>
@@ -3468,11 +3500,11 @@
       <c r="I82" t="s">
         <v>7</v>
       </c>
-      <c r="L82" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M82" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>94</v>
       </c>
@@ -3497,11 +3529,11 @@
       <c r="J83" t="s">
         <v>7</v>
       </c>
-      <c r="L83" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M83" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>95</v>
       </c>
@@ -3526,11 +3558,11 @@
       <c r="J84" t="s">
         <v>9</v>
       </c>
-      <c r="L84" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M84" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>96</v>
       </c>
@@ -3555,11 +3587,11 @@
       <c r="J85" t="s">
         <v>8</v>
       </c>
-      <c r="L85" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M85" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>97</v>
       </c>
@@ -3581,11 +3613,11 @@
       <c r="I86" t="s">
         <v>7</v>
       </c>
-      <c r="L86" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M86" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>98</v>
       </c>
@@ -3607,11 +3639,11 @@
       <c r="J87" t="s">
         <v>7</v>
       </c>
-      <c r="L87" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M87" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>99</v>
       </c>
@@ -3633,11 +3665,11 @@
       <c r="J88" t="s">
         <v>9</v>
       </c>
-      <c r="L88" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M88" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>100</v>
       </c>
@@ -3659,11 +3691,11 @@
       <c r="J89" t="s">
         <v>8</v>
       </c>
-      <c r="L89" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M89" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>101</v>
       </c>
@@ -3682,11 +3714,11 @@
       <c r="G90" t="s">
         <v>8</v>
       </c>
-      <c r="L90" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M90" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>102</v>
       </c>
@@ -3708,11 +3740,11 @@
       <c r="J91" t="s">
         <v>7</v>
       </c>
-      <c r="L91" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M91" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>103</v>
       </c>
@@ -3734,11 +3766,11 @@
       <c r="J92" t="s">
         <v>9</v>
       </c>
-      <c r="L92" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M92" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>104</v>
       </c>
@@ -3760,11 +3792,11 @@
       <c r="J93" t="s">
         <v>8</v>
       </c>
-      <c r="L93" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M93" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>105</v>
       </c>
@@ -3783,11 +3815,11 @@
       <c r="G94" t="s">
         <v>9</v>
       </c>
-      <c r="L94" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M94" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>106</v>
       </c>
@@ -3809,11 +3841,11 @@
       <c r="J95" t="s">
         <v>7</v>
       </c>
-      <c r="L95" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M95" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>107</v>
       </c>
@@ -3835,11 +3867,11 @@
       <c r="J96" t="s">
         <v>9</v>
       </c>
-      <c r="L96" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M96" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>108</v>
       </c>
@@ -3861,11 +3893,11 @@
       <c r="J97" t="s">
         <v>8</v>
       </c>
-      <c r="L97" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M97" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>109</v>
       </c>
@@ -3884,8 +3916,136 @@
       <c r="G98" t="s">
         <v>7</v>
       </c>
-      <c r="L98" t="s">
-        <v>110</v>
+      <c r="M98" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>120</v>
+      </c>
+      <c r="D99" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99" t="s">
+        <v>7</v>
+      </c>
+      <c r="F99" t="s">
+        <v>8</v>
+      </c>
+      <c r="G99" t="s">
+        <v>8</v>
+      </c>
+      <c r="H99" t="s">
+        <v>7</v>
+      </c>
+      <c r="I99" t="s">
+        <v>7</v>
+      </c>
+      <c r="J99" t="s">
+        <v>7</v>
+      </c>
+      <c r="K99" t="s">
+        <v>8</v>
+      </c>
+      <c r="M99" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>121</v>
+      </c>
+      <c r="D100" t="s">
+        <v>7</v>
+      </c>
+      <c r="E100" t="s">
+        <v>7</v>
+      </c>
+      <c r="F100" t="s">
+        <v>8</v>
+      </c>
+      <c r="G100" t="s">
+        <v>8</v>
+      </c>
+      <c r="H100" t="s">
+        <v>7</v>
+      </c>
+      <c r="I100" t="s">
+        <v>7</v>
+      </c>
+      <c r="K100" t="s">
+        <v>8</v>
+      </c>
+      <c r="M100" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>122</v>
+      </c>
+      <c r="B101" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" t="s">
+        <v>7</v>
+      </c>
+      <c r="E101" t="s">
+        <v>7</v>
+      </c>
+      <c r="F101" t="s">
+        <v>8</v>
+      </c>
+      <c r="G101" t="s">
+        <v>8</v>
+      </c>
+      <c r="H101" t="s">
+        <v>7</v>
+      </c>
+      <c r="I101" t="s">
+        <v>7</v>
+      </c>
+      <c r="J101" t="s">
+        <v>7</v>
+      </c>
+      <c r="K101" t="s">
+        <v>8</v>
+      </c>
+      <c r="M101" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>123</v>
+      </c>
+      <c r="B102" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102" t="s">
+        <v>7</v>
+      </c>
+      <c r="E102" t="s">
+        <v>7</v>
+      </c>
+      <c r="F102" t="s">
+        <v>8</v>
+      </c>
+      <c r="G102" t="s">
+        <v>8</v>
+      </c>
+      <c r="H102" t="s">
+        <v>7</v>
+      </c>
+      <c r="I102" t="s">
+        <v>7</v>
+      </c>
+      <c r="K102" t="s">
+        <v>8</v>
+      </c>
+      <c r="M102" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test cases acc101 to acc104
</commit_message>
<xml_diff>
--- a/validation/insurance_account_test_case_list.xlsx
+++ b/validation/insurance_account_test_case_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_fm_pol_cov_tests\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_account_terms\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAA8CB0-154E-4A35-81F4-A7702EF2E8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64CFBCB-1F93-4F77-866F-9689F30F2EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="780" windowWidth="22044" windowHeight="12384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="insurance_account" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="129">
   <si>
     <t>LocDed6All</t>
   </si>
@@ -408,6 +408,18 @@
   </si>
   <si>
     <t>complete</t>
+  </si>
+  <si>
+    <t>acc101</t>
+  </si>
+  <si>
+    <t>acc102</t>
+  </si>
+  <si>
+    <t>acc103</t>
+  </si>
+  <si>
+    <t>acc104</t>
   </si>
 </sst>
 </file>
@@ -958,9 +970,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -998,7 +1010,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1104,7 +1116,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1246,7 +1258,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1254,11 +1266,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P102"/>
+  <dimension ref="A1:P106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4048,6 +4058,74 @@
         <v>124</v>
       </c>
     </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>125</v>
+      </c>
+      <c r="D103" t="s">
+        <v>7</v>
+      </c>
+      <c r="E103" t="s">
+        <v>7</v>
+      </c>
+      <c r="F103" t="s">
+        <v>8</v>
+      </c>
+      <c r="K103" t="s">
+        <v>8</v>
+      </c>
+      <c r="M103" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>126</v>
+      </c>
+      <c r="K104" t="s">
+        <v>8</v>
+      </c>
+      <c r="M104" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>127</v>
+      </c>
+      <c r="B105" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105" t="s">
+        <v>7</v>
+      </c>
+      <c r="E105" t="s">
+        <v>7</v>
+      </c>
+      <c r="F105" t="s">
+        <v>8</v>
+      </c>
+      <c r="K105" t="s">
+        <v>8</v>
+      </c>
+      <c r="M105" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>128</v>
+      </c>
+      <c r="B106" t="s">
+        <v>7</v>
+      </c>
+      <c r="K106" t="s">
+        <v>8</v>
+      </c>
+      <c r="M106" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Feature/add fm tests (#1464)
* added test cases acc101 to acc104

* added tests sc18 and sc19

---------

Co-authored-by: Sam Gamble <hexadessa@gmail.com>
</commit_message>
<xml_diff>
--- a/validation/insurance_account_test_case_list.xlsx
+++ b/validation/insurance_account_test_case_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_fm_pol_cov_tests\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\OasisLMF_account_terms\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAA8CB0-154E-4A35-81F4-A7702EF2E8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64CFBCB-1F93-4F77-866F-9689F30F2EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="780" windowWidth="22044" windowHeight="12384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="insurance_account" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="129">
   <si>
     <t>LocDed6All</t>
   </si>
@@ -408,6 +408,18 @@
   </si>
   <si>
     <t>complete</t>
+  </si>
+  <si>
+    <t>acc101</t>
+  </si>
+  <si>
+    <t>acc102</t>
+  </si>
+  <si>
+    <t>acc103</t>
+  </si>
+  <si>
+    <t>acc104</t>
   </si>
 </sst>
 </file>
@@ -958,9 +970,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -998,7 +1010,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1104,7 +1116,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1246,7 +1258,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1254,11 +1266,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P102"/>
+  <dimension ref="A1:P106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4048,6 +4058,74 @@
         <v>124</v>
       </c>
     </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>125</v>
+      </c>
+      <c r="D103" t="s">
+        <v>7</v>
+      </c>
+      <c r="E103" t="s">
+        <v>7</v>
+      </c>
+      <c r="F103" t="s">
+        <v>8</v>
+      </c>
+      <c r="K103" t="s">
+        <v>8</v>
+      </c>
+      <c r="M103" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>126</v>
+      </c>
+      <c r="K104" t="s">
+        <v>8</v>
+      </c>
+      <c r="M104" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>127</v>
+      </c>
+      <c r="B105" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105" t="s">
+        <v>7</v>
+      </c>
+      <c r="E105" t="s">
+        <v>7</v>
+      </c>
+      <c r="F105" t="s">
+        <v>8</v>
+      </c>
+      <c r="K105" t="s">
+        <v>8</v>
+      </c>
+      <c r="M105" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>128</v>
+      </c>
+      <c r="B106" t="s">
+        <v>7</v>
+      </c>
+      <c r="K106" t="s">
+        <v>8</v>
+      </c>
+      <c r="M106" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>